<commit_message>
Refactored CsvReader + added ExcelReader
</commit_message>
<xml_diff>
--- a/src/UniqueFileRecordsComparer/tests/UniqueFileRecordsComparer.Core.IntegrationTests/TestFiles/OneFieldXlsxWithHeaders.xlsx
+++ b/src/UniqueFileRecordsComparer/tests/UniqueFileRecordsComparer.Core.IntegrationTests/TestFiles/OneFieldXlsxWithHeaders.xlsx
@@ -20,10 +20,10 @@
     <t>Nr</t>
   </si>
   <si>
-    <t>Naam</t>
-  </si>
-  <si>
-    <t>Adres</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Address</t>
   </si>
   <si>
     <t>New name</t>
@@ -408,7 +408,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>